<commit_message>
UML.html New Document in Specification
</commit_message>
<xml_diff>
--- a/Specification/Project Description.xlsx
+++ b/Specification/Project Description.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12340" yWindow="0" windowWidth="15820" windowHeight="16060" tabRatio="753" firstSheet="13" activeTab="18"/>
+    <workbookView xWindow="18340" yWindow="0" windowWidth="18560" windowHeight="16060" tabRatio="906" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="AudioPlayer" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="249">
   <si>
     <t>Variables</t>
   </si>
@@ -745,6 +745,45 @@
   </si>
   <si>
     <t>updateAvailableBingos()</t>
+  </si>
+  <si>
+    <t>plays clip once</t>
+  </si>
+  <si>
+    <t>plays clip repeatedly</t>
+  </si>
+  <si>
+    <t>stops clip</t>
+  </si>
+  <si>
+    <t>stops and closes clip</t>
+  </si>
+  <si>
+    <t>opens a music file with clip and sets volume</t>
+  </si>
+  <si>
+    <t>initializes the BallTicker</t>
+  </si>
+  <si>
+    <t>moves all balls 1 px to the right</t>
+  </si>
+  <si>
+    <t>adds n balls to the BallTicker and puts the numbers of the balls on the mc</t>
+  </si>
+  <si>
+    <t>creates a ball with number n</t>
+  </si>
+  <si>
+    <t>getNumberOfPlayerCards()</t>
+  </si>
+  <si>
+    <t>returns totalPlayerCards</t>
+  </si>
+  <si>
+    <t>returns "Cooper Black" if possible else returns "Impact"</t>
+  </si>
+  <si>
+    <t>Abstract method for adding the proper number of cells, numbers, cell behavior.</t>
   </si>
 </sst>
 </file>
@@ -1196,14 +1235,14 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="18">
@@ -1233,25 +1272,40 @@
       <c r="E3" t="s">
         <v>46</v>
       </c>
+      <c r="F3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="E4" t="s">
         <v>47</v>
       </c>
+      <c r="F4" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="E5" t="s">
         <v>48</v>
       </c>
+      <c r="F5" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="E6" t="s">
         <v>49</v>
       </c>
+      <c r="F6" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="E7" t="s">
         <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2122,7 +2176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
@@ -2198,7 +2252,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2207,7 +2261,7 @@
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="18">
@@ -2237,6 +2291,9 @@
       <c r="E3" t="s">
         <v>85</v>
       </c>
+      <c r="F3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -2248,6 +2305,9 @@
       <c r="E4" t="s">
         <v>86</v>
       </c>
+      <c r="F4" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
@@ -2258,6 +2318,9 @@
       </c>
       <c r="E5" t="s">
         <v>87</v>
+      </c>
+      <c r="F5" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2511,7 +2574,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2519,8 +2582,8 @@
     <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="18">
@@ -2561,6 +2624,9 @@
       <c r="E4" t="s">
         <v>72</v>
       </c>
+      <c r="F4" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
@@ -2570,7 +2636,10 @@
         <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>245</v>
+      </c>
+      <c r="F5" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2579,6 +2648,12 @@
       </c>
       <c r="B6" t="s">
         <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2670,7 +2745,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2678,7 +2753,7 @@
     <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="18">
@@ -2718,6 +2793,9 @@
       </c>
       <c r="E4" t="s">
         <v>99</v>
+      </c>
+      <c r="F4" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2774,9 +2852,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>